<commit_message>
fin output ticket page
</commit_message>
<xml_diff>
--- a/public/excel/writed_form1-1.xlsx
+++ b/public/excel/writed_form1-1.xlsx
@@ -13873,11 +13873,11 @@
         <v>1</v>
       </c>
       <c r="J37" s="2" t="str">
-        <v>木</v>
+        <v>土</v>
       </c>
       <c r="K37" s="366"/>
       <c r="L37" s="2" t="str">
-        <v>2023-05-11 10:41</v>
+        <v>2023-04-01 16:40</v>
       </c>
       <c r="M37" s="583"/>
       <c r="N37" s="583"/>
@@ -13886,13 +13886,13 @@
         <v>65</v>
       </c>
       <c r="Q37" s="2" t="str">
-        <v>2023-05-11 13:42</v>
+        <v>2023-04-01 20:40</v>
       </c>
       <c r="R37" s="580"/>
       <c r="S37" s="580"/>
       <c r="T37" s="581"/>
       <c r="U37" s="2">
-        <v>12</v>
+        <v>150</v>
       </c>
       <c r="V37" s="583"/>
       <c r="W37" s="583"/>
@@ -13923,11 +13923,11 @@
         <v>1</v>
       </c>
       <c r="J38" s="2" t="str">
-        <v>金</v>
+        <v>木</v>
       </c>
       <c r="K38" s="293"/>
       <c r="L38" s="2" t="str">
-        <v>2023-07-07 10:21</v>
+        <v>2023-05-11 10:41</v>
       </c>
       <c r="M38" s="590"/>
       <c r="N38" s="590"/>
@@ -13936,13 +13936,13 @@
         <v>65</v>
       </c>
       <c r="Q38" s="2" t="str">
-        <v>2023-07-07 14:21</v>
+        <v>2023-05-11 13:42</v>
       </c>
       <c r="R38" s="590"/>
       <c r="S38" s="590"/>
       <c r="T38" s="591"/>
       <c r="U38" s="2">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="V38" s="590"/>
       <c r="W38" s="590"/>
@@ -13973,11 +13973,11 @@
         <v>1</v>
       </c>
       <c r="J39" s="2" t="str">
-        <v>水</v>
+        <v>金</v>
       </c>
       <c r="K39" s="579"/>
       <c r="L39" s="2" t="str">
-        <v>2023-07-12 12:20</v>
+        <v>2023-07-07 10:21</v>
       </c>
       <c r="M39" s="572"/>
       <c r="N39" s="572"/>
@@ -13986,13 +13986,13 @@
         <v>65</v>
       </c>
       <c r="Q39" s="2" t="str">
-        <v>2023-07-12 13:20</v>
+        <v>2023-07-07 14:21</v>
       </c>
       <c r="R39" s="572"/>
       <c r="S39" s="572"/>
       <c r="T39" s="573"/>
       <c r="U39" s="2">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="V39" s="572"/>
       <c r="W39" s="572"/>
@@ -14023,11 +14023,11 @@
         <v>1</v>
       </c>
       <c r="J40" s="2" t="str">
-        <v>木</v>
+        <v>水</v>
       </c>
       <c r="K40" s="366"/>
       <c r="L40" s="2" t="str">
-        <v>2023-07-13 12:42</v>
+        <v>2023-07-12 15:36</v>
       </c>
       <c r="M40" s="604"/>
       <c r="N40" s="604"/>
@@ -14036,13 +14036,13 @@
         <v>65</v>
       </c>
       <c r="Q40" s="2" t="str">
-        <v>2023-07-13 14:45</v>
+        <v>2023-07-12 19:36</v>
       </c>
       <c r="R40" s="601"/>
       <c r="S40" s="601"/>
       <c r="T40" s="602"/>
       <c r="U40" s="2">
-        <v>10</v>
+        <v>200</v>
       </c>
       <c r="V40" s="604"/>
       <c r="W40" s="604"/>
@@ -14073,11 +14073,11 @@
         <v>1</v>
       </c>
       <c r="J41" s="2" t="str">
-        <v>金</v>
+        <v>木</v>
       </c>
       <c r="K41" s="293"/>
       <c r="L41" s="2" t="str">
-        <v>2023-07-14 10:32</v>
+        <v>2023-07-13 12:42</v>
       </c>
       <c r="M41" s="590"/>
       <c r="N41" s="590"/>
@@ -14086,7 +14086,7 @@
         <v>65</v>
       </c>
       <c r="Q41" s="2" t="str">
-        <v>2023-07-14 15:32</v>
+        <v>2023-07-13 14:45</v>
       </c>
       <c r="R41" s="590"/>
       <c r="S41" s="590"/>
@@ -14123,11 +14123,11 @@
         <v>1</v>
       </c>
       <c r="J42" s="2" t="str">
-        <v>木</v>
+        <v>金</v>
       </c>
       <c r="K42" s="579"/>
       <c r="L42" s="2" t="str">
-        <v>2023-07-20 10:32</v>
+        <v>2023-07-14 10:32</v>
       </c>
       <c r="M42" s="572"/>
       <c r="N42" s="572"/>
@@ -14136,13 +14136,13 @@
         <v>65</v>
       </c>
       <c r="Q42" s="2" t="str">
-        <v>2023-07-20 14:32</v>
+        <v>2023-07-14 15:32</v>
       </c>
       <c r="R42" s="610"/>
       <c r="S42" s="610"/>
       <c r="T42" s="611"/>
       <c r="U42" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="V42" s="572"/>
       <c r="W42" s="572"/>
@@ -14177,7 +14177,7 @@
       </c>
       <c r="K43" s="366"/>
       <c r="L43" s="2" t="str">
-        <v>2023-07-20 11:22</v>
+        <v>2023-07-20 10:32</v>
       </c>
       <c r="M43" s="604"/>
       <c r="N43" s="604"/>
@@ -14186,13 +14186,13 @@
         <v>65</v>
       </c>
       <c r="Q43" s="2" t="str">
-        <v>2023-07-20 13:22</v>
+        <v>2023-07-20 14:32</v>
       </c>
       <c r="R43" s="601"/>
       <c r="S43" s="601"/>
       <c r="T43" s="602"/>
       <c r="U43" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="V43" s="604"/>
       <c r="W43" s="604"/>
@@ -14223,11 +14223,11 @@
         <v>1</v>
       </c>
       <c r="J44" s="2" t="str">
-        <v>金</v>
+        <v>木</v>
       </c>
       <c r="K44" s="293"/>
       <c r="L44" s="2" t="str">
-        <v>2023-07-21 10:23</v>
+        <v>2023-07-20 11:22</v>
       </c>
       <c r="M44" s="590"/>
       <c r="N44" s="590"/>
@@ -14236,13 +14236,13 @@
         <v>65</v>
       </c>
       <c r="Q44" s="2" t="str">
-        <v>2023-07-28 10:26</v>
+        <v>2023-07-20 13:22</v>
       </c>
       <c r="R44" s="590"/>
       <c r="S44" s="590"/>
       <c r="T44" s="591"/>
       <c r="U44" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="V44" s="590"/>
       <c r="W44" s="590"/>
@@ -14277,7 +14277,7 @@
       </c>
       <c r="K45" s="579"/>
       <c r="L45" s="2" t="str">
-        <v>2023-07-21 10:42</v>
+        <v>2023-07-21 10:23</v>
       </c>
       <c r="M45" s="572"/>
       <c r="N45" s="572"/>
@@ -14286,13 +14286,13 @@
         <v>65</v>
       </c>
       <c r="Q45" s="2" t="str">
-        <v>2023-07-21 14:42</v>
+        <v>2023-07-28 10:26</v>
       </c>
       <c r="R45" s="572"/>
       <c r="S45" s="572"/>
       <c r="T45" s="573"/>
       <c r="U45" s="2">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="V45" s="572"/>
       <c r="W45" s="572"/>
@@ -14323,11 +14323,11 @@
         <v>1</v>
       </c>
       <c r="J46" s="2" t="str">
-        <v>土</v>
+        <v>金</v>
       </c>
       <c r="K46" s="366"/>
       <c r="L46" s="2" t="str">
-        <v>2023-07-22 10:44</v>
+        <v>2023-07-21 10:42</v>
       </c>
       <c r="M46" s="604"/>
       <c r="N46" s="604"/>
@@ -14336,13 +14336,13 @@
         <v>65</v>
       </c>
       <c r="Q46" s="2" t="str">
-        <v>2023-07-22 10:49</v>
+        <v>2023-07-21 14:42</v>
       </c>
       <c r="R46" s="601"/>
       <c r="S46" s="601"/>
       <c r="T46" s="602"/>
       <c r="U46" s="2">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="V46" s="604"/>
       <c r="W46" s="604"/>
@@ -14373,11 +14373,11 @@
         <v>1</v>
       </c>
       <c r="J47" s="2" t="str">
-        <v>金</v>
+        <v>土</v>
       </c>
       <c r="K47" s="293"/>
       <c r="L47" s="2" t="str">
-        <v>2023-07-28 12:43</v>
+        <v>2023-07-22 10:44</v>
       </c>
       <c r="M47" s="590"/>
       <c r="N47" s="590"/>
@@ -14386,13 +14386,13 @@
         <v>65</v>
       </c>
       <c r="Q47" s="2" t="str">
-        <v>2023-07-28 15:43</v>
+        <v>2023-07-22 10:49</v>
       </c>
       <c r="R47" s="590"/>
       <c r="S47" s="590"/>
       <c r="T47" s="591"/>
       <c r="U47" s="2">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="V47" s="590"/>
       <c r="W47" s="590"/>
@@ -14423,11 +14423,11 @@
         <v>1</v>
       </c>
       <c r="J48" s="2" t="str">
-        <v>月</v>
+        <v>金</v>
       </c>
       <c r="K48" s="579"/>
       <c r="L48" s="2" t="str">
-        <v>2023-07-31 15:43</v>
+        <v>2023-07-28 12:43</v>
       </c>
       <c r="M48" s="572"/>
       <c r="N48" s="572"/>
@@ -14436,13 +14436,13 @@
         <v>65</v>
       </c>
       <c r="Q48" s="2" t="str">
-        <v>2023-07-31 16:43</v>
+        <v>2023-07-28 15:43</v>
       </c>
       <c r="R48" s="572"/>
       <c r="S48" s="572"/>
       <c r="T48" s="573"/>
       <c r="U48" s="2">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="V48" s="572"/>
       <c r="W48" s="572"/>
@@ -14459,25 +14459,25 @@
     <row r="49" spans="1:32" customFormat="false" ht="25.5" customHeight="1">
       <c r="A49" s="560"/>
       <c r="B49" s="2" t="str">
-        <v>090002</v>
+        <v>090001</v>
       </c>
       <c r="C49" s="597"/>
       <c r="D49" s="2" t="str">
-        <v>Course2</v>
+        <v>Course1</v>
       </c>
       <c r="E49" s="599"/>
       <c r="F49" s="599"/>
       <c r="G49" s="599"/>
       <c r="H49" s="600"/>
       <c r="I49" s="2" t="str">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J49" s="2" t="str">
-        <v>木</v>
+        <v>月</v>
       </c>
       <c r="K49" s="366"/>
       <c r="L49" s="2" t="str">
-        <v>2023-07-13 10:52</v>
+        <v>2023-07-31 15:43</v>
       </c>
       <c r="M49" s="604"/>
       <c r="N49" s="604"/>
@@ -14486,13 +14486,13 @@
         <v>65</v>
       </c>
       <c r="Q49" s="2" t="str">
-        <v>2023-07-13 13:52</v>
+        <v>2023-07-31 16:43</v>
       </c>
       <c r="R49" s="601"/>
       <c r="S49" s="601"/>
       <c r="T49" s="602"/>
       <c r="U49" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V49" s="604"/>
       <c r="W49" s="604"/>
@@ -14509,25 +14509,25 @@
     <row r="50" spans="1:32" customFormat="false" ht="25.5" customHeight="1">
       <c r="A50" s="560"/>
       <c r="B50" s="2" t="str">
-        <v>090002</v>
+        <v>090001</v>
       </c>
       <c r="C50" s="589"/>
       <c r="D50" s="2" t="str">
-        <v>Course2</v>
+        <v>Course1</v>
       </c>
       <c r="E50" s="295"/>
       <c r="F50" s="295"/>
       <c r="G50" s="295"/>
       <c r="H50" s="296"/>
       <c r="I50" s="2" t="str">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J50" s="2" t="str">
         <v>土</v>
       </c>
       <c r="K50" s="293"/>
       <c r="L50" s="2" t="str">
-        <v>2023-07-15 10:53</v>
+        <v>2024-03-30 16:39</v>
       </c>
       <c r="M50" s="590"/>
       <c r="N50" s="590"/>
@@ -14536,13 +14536,13 @@
         <v>65</v>
       </c>
       <c r="Q50" s="2" t="str">
-        <v>2023-07-15 14:53</v>
+        <v>2024-03-30 21:39</v>
       </c>
       <c r="R50" s="590"/>
       <c r="S50" s="590"/>
       <c r="T50" s="591"/>
       <c r="U50" s="2">
-        <v>3</v>
+        <v>200</v>
       </c>
       <c r="V50" s="590"/>
       <c r="W50" s="590"/>
@@ -14573,11 +14573,11 @@
         <v>2</v>
       </c>
       <c r="J51" s="2" t="str">
-        <v>金</v>
+        <v>木</v>
       </c>
       <c r="K51" s="625"/>
       <c r="L51" s="2" t="str">
-        <v>2023-07-21 10:53</v>
+        <v>2023-07-13 10:52</v>
       </c>
       <c r="M51" s="618"/>
       <c r="N51" s="618"/>
@@ -14586,13 +14586,13 @@
         <v>65</v>
       </c>
       <c r="Q51" s="2" t="str">
-        <v>2023-07-21 13:53</v>
+        <v>2023-07-13 13:52</v>
       </c>
       <c r="R51" s="618"/>
       <c r="S51" s="618"/>
       <c r="T51" s="619"/>
       <c r="U51" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="V51" s="618"/>
       <c r="W51" s="618"/>

</xml_diff>

<commit_message>
Fix output button link
</commit_message>
<xml_diff>
--- a/public/excel/writed_form1-1.xlsx
+++ b/public/excel/writed_form1-1.xlsx
@@ -13977,7 +13977,7 @@
       </c>
       <c r="K39" s="579"/>
       <c r="L39" s="2" t="str">
-        <v>2023-07-07 10:21</v>
+        <v>2023-06-30 20:43</v>
       </c>
       <c r="M39" s="572"/>
       <c r="N39" s="572"/>
@@ -13986,13 +13986,13 @@
         <v>65</v>
       </c>
       <c r="Q39" s="2" t="str">
-        <v>2023-07-07 14:21</v>
+        <v>2023-07-28 20:43</v>
       </c>
       <c r="R39" s="572"/>
       <c r="S39" s="572"/>
       <c r="T39" s="573"/>
       <c r="U39" s="2">
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="V39" s="572"/>
       <c r="W39" s="572"/>
@@ -14023,11 +14023,11 @@
         <v>1</v>
       </c>
       <c r="J40" s="2" t="str">
-        <v>水</v>
+        <v>金</v>
       </c>
       <c r="K40" s="366"/>
       <c r="L40" s="2" t="str">
-        <v>2023-07-12 15:36</v>
+        <v>2023-07-07 10:21</v>
       </c>
       <c r="M40" s="604"/>
       <c r="N40" s="604"/>
@@ -14036,13 +14036,13 @@
         <v>65</v>
       </c>
       <c r="Q40" s="2" t="str">
-        <v>2023-07-12 19:36</v>
+        <v>2023-07-07 14:21</v>
       </c>
       <c r="R40" s="601"/>
       <c r="S40" s="601"/>
       <c r="T40" s="602"/>
       <c r="U40" s="2">
-        <v>200</v>
+        <v>35</v>
       </c>
       <c r="V40" s="604"/>
       <c r="W40" s="604"/>
@@ -14073,11 +14073,11 @@
         <v>1</v>
       </c>
       <c r="J41" s="2" t="str">
-        <v>木</v>
+        <v>水</v>
       </c>
       <c r="K41" s="293"/>
       <c r="L41" s="2" t="str">
-        <v>2023-07-13 12:42</v>
+        <v>2023-07-12 15:36</v>
       </c>
       <c r="M41" s="590"/>
       <c r="N41" s="590"/>
@@ -14086,13 +14086,13 @@
         <v>65</v>
       </c>
       <c r="Q41" s="2" t="str">
-        <v>2023-07-13 14:45</v>
+        <v>2023-07-12 19:36</v>
       </c>
       <c r="R41" s="590"/>
       <c r="S41" s="590"/>
       <c r="T41" s="591"/>
       <c r="U41" s="2">
-        <v>10</v>
+        <v>200</v>
       </c>
       <c r="V41" s="590"/>
       <c r="W41" s="590"/>
@@ -14123,11 +14123,11 @@
         <v>1</v>
       </c>
       <c r="J42" s="2" t="str">
-        <v>金</v>
+        <v>木</v>
       </c>
       <c r="K42" s="579"/>
       <c r="L42" s="2" t="str">
-        <v>2023-07-14 10:32</v>
+        <v>2023-07-13 12:42</v>
       </c>
       <c r="M42" s="572"/>
       <c r="N42" s="572"/>
@@ -14136,7 +14136,7 @@
         <v>65</v>
       </c>
       <c r="Q42" s="2" t="str">
-        <v>2023-07-14 15:32</v>
+        <v>2023-07-13 14:45</v>
       </c>
       <c r="R42" s="610"/>
       <c r="S42" s="610"/>
@@ -14173,11 +14173,11 @@
         <v>1</v>
       </c>
       <c r="J43" s="2" t="str">
-        <v>木</v>
+        <v>金</v>
       </c>
       <c r="K43" s="366"/>
       <c r="L43" s="2" t="str">
-        <v>2023-07-20 10:32</v>
+        <v>2023-07-14 10:32</v>
       </c>
       <c r="M43" s="604"/>
       <c r="N43" s="604"/>
@@ -14186,13 +14186,13 @@
         <v>65</v>
       </c>
       <c r="Q43" s="2" t="str">
-        <v>2023-07-20 14:32</v>
+        <v>2023-07-14 15:32</v>
       </c>
       <c r="R43" s="601"/>
       <c r="S43" s="601"/>
       <c r="T43" s="602"/>
       <c r="U43" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="V43" s="604"/>
       <c r="W43" s="604"/>
@@ -14227,7 +14227,7 @@
       </c>
       <c r="K44" s="293"/>
       <c r="L44" s="2" t="str">
-        <v>2023-07-20 11:22</v>
+        <v>2023-07-20 10:32</v>
       </c>
       <c r="M44" s="590"/>
       <c r="N44" s="590"/>
@@ -14236,13 +14236,13 @@
         <v>65</v>
       </c>
       <c r="Q44" s="2" t="str">
-        <v>2023-07-20 13:22</v>
+        <v>2023-07-20 14:32</v>
       </c>
       <c r="R44" s="590"/>
       <c r="S44" s="590"/>
       <c r="T44" s="591"/>
       <c r="U44" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="V44" s="590"/>
       <c r="W44" s="590"/>
@@ -14273,11 +14273,11 @@
         <v>1</v>
       </c>
       <c r="J45" s="2" t="str">
-        <v>金</v>
+        <v>木</v>
       </c>
       <c r="K45" s="579"/>
       <c r="L45" s="2" t="str">
-        <v>2023-07-21 10:23</v>
+        <v>2023-07-20 11:22</v>
       </c>
       <c r="M45" s="572"/>
       <c r="N45" s="572"/>
@@ -14286,13 +14286,13 @@
         <v>65</v>
       </c>
       <c r="Q45" s="2" t="str">
-        <v>2023-07-28 10:26</v>
+        <v>2023-07-20 13:22</v>
       </c>
       <c r="R45" s="572"/>
       <c r="S45" s="572"/>
       <c r="T45" s="573"/>
       <c r="U45" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="V45" s="572"/>
       <c r="W45" s="572"/>
@@ -14327,7 +14327,7 @@
       </c>
       <c r="K46" s="366"/>
       <c r="L46" s="2" t="str">
-        <v>2023-07-21 10:42</v>
+        <v>2023-07-21 10:23</v>
       </c>
       <c r="M46" s="604"/>
       <c r="N46" s="604"/>
@@ -14336,13 +14336,13 @@
         <v>65</v>
       </c>
       <c r="Q46" s="2" t="str">
-        <v>2023-07-21 14:42</v>
+        <v>2023-07-28 10:26</v>
       </c>
       <c r="R46" s="601"/>
       <c r="S46" s="601"/>
       <c r="T46" s="602"/>
       <c r="U46" s="2">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="V46" s="604"/>
       <c r="W46" s="604"/>
@@ -14373,11 +14373,11 @@
         <v>1</v>
       </c>
       <c r="J47" s="2" t="str">
-        <v>土</v>
+        <v>金</v>
       </c>
       <c r="K47" s="293"/>
       <c r="L47" s="2" t="str">
-        <v>2023-07-22 10:44</v>
+        <v>2023-07-21 10:42</v>
       </c>
       <c r="M47" s="590"/>
       <c r="N47" s="590"/>
@@ -14386,13 +14386,13 @@
         <v>65</v>
       </c>
       <c r="Q47" s="2" t="str">
-        <v>2023-07-22 10:49</v>
+        <v>2023-07-21 14:42</v>
       </c>
       <c r="R47" s="590"/>
       <c r="S47" s="590"/>
       <c r="T47" s="591"/>
       <c r="U47" s="2">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="V47" s="590"/>
       <c r="W47" s="590"/>
@@ -14423,11 +14423,11 @@
         <v>1</v>
       </c>
       <c r="J48" s="2" t="str">
-        <v>金</v>
+        <v>土</v>
       </c>
       <c r="K48" s="579"/>
       <c r="L48" s="2" t="str">
-        <v>2023-07-28 12:43</v>
+        <v>2023-07-22 10:44</v>
       </c>
       <c r="M48" s="572"/>
       <c r="N48" s="572"/>
@@ -14436,13 +14436,13 @@
         <v>65</v>
       </c>
       <c r="Q48" s="2" t="str">
-        <v>2023-07-28 15:43</v>
+        <v>2023-07-22 10:49</v>
       </c>
       <c r="R48" s="572"/>
       <c r="S48" s="572"/>
       <c r="T48" s="573"/>
       <c r="U48" s="2">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="V48" s="572"/>
       <c r="W48" s="572"/>
@@ -14473,11 +14473,11 @@
         <v>1</v>
       </c>
       <c r="J49" s="2" t="str">
-        <v>月</v>
+        <v>金</v>
       </c>
       <c r="K49" s="366"/>
       <c r="L49" s="2" t="str">
-        <v>2023-07-31 15:43</v>
+        <v>2023-07-28 12:43</v>
       </c>
       <c r="M49" s="604"/>
       <c r="N49" s="604"/>
@@ -14486,13 +14486,13 @@
         <v>65</v>
       </c>
       <c r="Q49" s="2" t="str">
-        <v>2023-07-31 16:43</v>
+        <v>2023-07-28 15:43</v>
       </c>
       <c r="R49" s="601"/>
       <c r="S49" s="601"/>
       <c r="T49" s="602"/>
       <c r="U49" s="2">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="V49" s="604"/>
       <c r="W49" s="604"/>
@@ -14523,11 +14523,11 @@
         <v>1</v>
       </c>
       <c r="J50" s="2" t="str">
-        <v>土</v>
+        <v>月</v>
       </c>
       <c r="K50" s="293"/>
       <c r="L50" s="2" t="str">
-        <v>2024-03-30 16:39</v>
+        <v>2023-07-31 15:43</v>
       </c>
       <c r="M50" s="590"/>
       <c r="N50" s="590"/>
@@ -14536,13 +14536,13 @@
         <v>65</v>
       </c>
       <c r="Q50" s="2" t="str">
-        <v>2024-03-30 21:39</v>
+        <v>2023-07-31 16:43</v>
       </c>
       <c r="R50" s="590"/>
       <c r="S50" s="590"/>
       <c r="T50" s="591"/>
       <c r="U50" s="2">
-        <v>200</v>
+        <v>4</v>
       </c>
       <c r="V50" s="590"/>
       <c r="W50" s="590"/>
@@ -14559,25 +14559,25 @@
     <row r="51" spans="1:32" customFormat="false" ht="25.5" customHeight="1" thickBot="1">
       <c r="A51" s="561"/>
       <c r="B51" s="2" t="str">
-        <v>090002</v>
+        <v>090001</v>
       </c>
       <c r="C51" s="614"/>
       <c r="D51" s="2" t="str">
-        <v>Course2</v>
+        <v>Course1</v>
       </c>
       <c r="E51" s="616"/>
       <c r="F51" s="616"/>
       <c r="G51" s="616"/>
       <c r="H51" s="617"/>
       <c r="I51" s="2" t="str">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J51" s="2" t="str">
-        <v>木</v>
+        <v>土</v>
       </c>
       <c r="K51" s="625"/>
       <c r="L51" s="2" t="str">
-        <v>2023-07-13 10:52</v>
+        <v>2024-03-30 16:39</v>
       </c>
       <c r="M51" s="618"/>
       <c r="N51" s="618"/>
@@ -14586,13 +14586,13 @@
         <v>65</v>
       </c>
       <c r="Q51" s="2" t="str">
-        <v>2023-07-13 13:52</v>
+        <v>2024-03-30 21:39</v>
       </c>
       <c r="R51" s="618"/>
       <c r="S51" s="618"/>
       <c r="T51" s="619"/>
       <c r="U51" s="2">
-        <v>2</v>
+        <v>200</v>
       </c>
       <c r="V51" s="618"/>
       <c r="W51" s="618"/>

</xml_diff>

<commit_message>
fix login error, button size, top-page-layout
</commit_message>
<xml_diff>
--- a/public/excel/writed_form1-1.xlsx
+++ b/public/excel/writed_form1-1.xlsx
@@ -13873,11 +13873,11 @@
         <v>2</v>
       </c>
       <c r="J37" s="2" t="str">
-        <v>日</v>
+        <v>木</v>
       </c>
       <c r="K37" s="366"/>
       <c r="L37" s="2" t="str">
-        <v>2023-07-16 16:12</v>
+        <v>2023-07-20 16:12</v>
       </c>
       <c r="M37" s="583"/>
       <c r="N37" s="583"/>
@@ -13886,7 +13886,7 @@
         <v>65</v>
       </c>
       <c r="Q37" s="2" t="str">
-        <v>2023-07-16 17:12</v>
+        <v>2023-07-20 17:12</v>
       </c>
       <c r="R37" s="580"/>
       <c r="S37" s="580"/>

</xml_diff>